<commit_message>
Cobranzas por cabecera base y Marca reporte Efectores
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Efectores/tabla_parametros_comprobantes.xlsx
+++ b/DBA/Reportes BI/2021/Efectores/tabla_parametros_comprobantes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\FACOEP\DBA\Reportes BI\2021\Efectores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iachenbach\Gobierno de la Ciudad de Buenos Aires\Pablo Alfredo Gadea - Tablero Facoep P BI\FACOEP\DBA\Reportes BI\2021\Efectores\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>FACA2</t>
   </si>
@@ -78,6 +78,18 @@
   </si>
   <si>
     <t>notadb</t>
+  </si>
+  <si>
+    <t>NCA</t>
+  </si>
+  <si>
+    <t>NCB</t>
+  </si>
+  <si>
+    <t>NCECA</t>
+  </si>
+  <si>
+    <t>notacredito</t>
   </si>
 </sst>
 </file>
@@ -174,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -199,6 +211,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -256,8 +271,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tabla_parametros_comprobantes" displayName="tabla_parametros_comprobantes" ref="A1:B14" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="A1:B14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tabla_parametros_comprobantes" displayName="tabla_parametros_comprobantes" ref="A1:B17" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="A1:B17"/>
   <tableColumns count="2">
     <tableColumn id="2" name="Comprobante" dataDxfId="1"/>
     <tableColumn id="1" name="tipo" dataDxfId="0"/>
@@ -529,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,6 +669,30 @@
         <v>17</v>
       </c>
     </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>